<commit_message>
Corrected the user verification
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -1,49 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\king\OneDrive\Desktop\Master_1\Online-Voting-System-using-python\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F8C014-9DFE-443D-8450-746057448280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Election_ID</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Flag</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="3">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,7 +62,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -64,16 +79,48 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -211,7 +258,6 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
@@ -222,27 +268,31 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
@@ -264,7 +314,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -322,7 +372,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -335,13 +385,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -353,148 +402,228 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Election_ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>DOB</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Flag</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
         <v>1234567890</v>
       </c>
-      <c r="B2" t="str">
-        <v>2005/03/24</v>
-      </c>
-      <c r="C2" t="str">
+      <c r="B2" s="5">
+        <v>38435</v>
+      </c>
+      <c r="C2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
+    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>1234567899</v>
       </c>
-      <c r="B3" t="str">
-        <v>2005/03/23</v>
-      </c>
-      <c r="C3" t="str">
+      <c r="B3" s="5">
+        <v>38434</v>
+      </c>
+      <c r="C3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
+    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
         <v>1234567898</v>
       </c>
-      <c r="B4" t="str">
-        <v>2005/03/22</v>
-      </c>
-      <c r="C4" t="str">
+      <c r="B4" s="5">
+        <v>38433</v>
+      </c>
+      <c r="C4" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>1,234,567,890</v>
-      </c>
-      <c r="B27" t="str">
-        <v>1970-01-01 5:30:26</v>
-      </c>
-      <c r="C27" t="str">
+    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="B27" s="2">
+        <v>25569.229462604169</v>
+      </c>
+      <c r="C27" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="str">
-        <v>1,234,567,890</v>
-      </c>
-      <c r="B28" t="str">
-        <v>1970-01-01 5:30:26</v>
-      </c>
-      <c r="C28" t="str">
+    <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="B28" s="2">
+        <v>25569.229462604169</v>
+      </c>
+      <c r="C28" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="str">
-        <v>1,234,567,890</v>
-      </c>
-      <c r="B29" t="str">
-        <v>1970-01-01 5:30:26</v>
-      </c>
-      <c r="C29" t="str">
+    <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="B29" s="2">
+        <v>25569.229462604169</v>
+      </c>
+      <c r="C29" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="str">
-        <v>1,234,567,899</v>
-      </c>
-      <c r="B30" t="str">
-        <v>1970-01-01 5:30:26</v>
-      </c>
-      <c r="C30" t="str">
+    <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>1234567899</v>
+      </c>
+      <c r="B30" s="6">
+        <v>25569.229462604169</v>
+      </c>
+      <c r="C30" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C30"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>